<commit_message>
Modificación del archivo XLSX
</commit_message>
<xml_diff>
--- a/trackingKW.xlsx
+++ b/trackingKW.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jeshua\Desktop\Portfolio\Proyectos\SERP_Tracker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F29D04C6-D3C4-490A-B3E4-B347B9820728}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E858629B-1600-4AD2-A151-4DEA33D25F37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>es</t>
   </si>
@@ -55,9 +55,6 @@
   </si>
   <si>
     <t>keyword5</t>
-  </si>
-  <si>
-    <t>keyword6</t>
   </si>
 </sst>
 </file>
@@ -407,10 +404,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -462,11 +459,6 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C7" t="s">
-        <v>10</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>